<commit_message>
a++1 a++10 a++b 추가함
</commit_message>
<xml_diff>
--- a/inputCode.xlsx
+++ b/inputCode.xlsx
@@ -3,14 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eclipse\Compiler\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D5EC5D-4B3B-4D8B-8631-CC5871E22687}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{86B8AC19-E1E5-4B3B-AED4-62F140AE75FC}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="13096" xr2:uid="{31C4744E-66A6-4566-A74E-ACB3BF1E5F9A}"/>
+    <workbookView xWindow="1470" yWindow="1470" windowWidth="24210" windowHeight="13725" xr2:uid="{31C4744E-66A6-4566-A74E-ACB3BF1E5F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="1. code exam" sheetId="1" r:id="rId1"/>
@@ -21,6 +16,7 @@
     <sheet name="example" sheetId="4" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -1475,10 +1471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2A8671B-8ADF-44B6-95FD-28323871EB5E}">
-  <dimension ref="A1:G47"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.899999999999999" x14ac:dyDescent="0.6"/>
@@ -2133,6 +2129,7 @@
       </c>
       <c r="G47" s="57"/>
     </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.6"/>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>